<commit_message>
det and algebra cofactor add
</commit_message>
<xml_diff>
--- a/backschool.xlsx
+++ b/backschool.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>茅傲岳</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -255,6 +255,26 @@
   </si>
   <si>
     <t>茅傲岳 董芮江</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18日午间十分钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19日午间十分钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向东伟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邓涵朵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陶昱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -312,10 +332,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,7 +620,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:J13"/>
+      <selection activeCell="H6" sqref="H6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -615,12 +635,12 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -632,9 +652,9 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="1" t="s">
         <v>41</v>
       </c>
@@ -649,11 +669,11 @@
       <c r="G3" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="1" t="s">
         <v>42</v>
       </c>
@@ -668,13 +688,15 @@
       <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -686,11 +708,15 @@
       <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -705,11 +731,11 @@
       <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="1" t="s">
         <v>43</v>
       </c>
@@ -724,11 +750,15 @@
       <c r="G7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -743,11 +773,11 @@
       <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="1" t="s">
         <v>44</v>
       </c>
@@ -765,11 +795,11 @@
       <c r="G9" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="1" t="s">
         <v>45</v>
       </c>
@@ -784,11 +814,11 @@
       <c r="G10" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="1" t="s">
         <v>46</v>
       </c>
@@ -803,11 +833,11 @@
       <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="1" t="s">
         <v>47</v>
       </c>
@@ -816,11 +846,11 @@
       <c r="G12" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="1" t="s">
         <v>48</v>
       </c>
@@ -829,11 +859,11 @@
       <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="1" t="s">
         <v>49</v>
       </c>
@@ -842,11 +872,11 @@
       <c r="G14" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="1" t="s">
         <v>50</v>
       </c>
@@ -858,37 +888,47 @@
       <c r="G15" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
       <c r="K15" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="H10:J10"/>
@@ -899,16 +939,6 @@
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>